<commit_message>
Inserito il file di pratica extra
</commit_message>
<xml_diff>
--- a/ESERCIZIO_M2-1-1_dati.xlsx
+++ b/ESERCIZIO_M2-1-1_dati.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/066615358B04905F/08 -  Workspace/EPICODE - Data Analyst/M1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\melli\Documents\1 - Workspace\EPICODE\DAPT0824-W1-funzioni-logiche-e-di-ricerca\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="11_B4F75B78FD140C97F52DC8033C40F348BD2C39D9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6856F44-4101-42C5-ACD1-5BCC4C99E003}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEAC0AFC-FB32-459A-8CC8-646D06B6C430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1975,8 +1975,8 @@
         <vertAlign val="baseline"/>
         <sz val="10"/>
         <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
       </font>
     </dxf>
     <dxf>
@@ -2026,8 +2026,8 @@
         <vertAlign val="baseline"/>
         <sz val="10"/>
         <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
       </font>
     </dxf>
     <dxf>
@@ -2114,11 +2114,11 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A722E349-13CC-4819-B8D7-4822A079EA8B}" name="Table2" displayName="Table2" ref="G1:H5" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A722E349-13CC-4819-B8D7-4822A079EA8B}" name="Table2" displayName="Table2" ref="G1:H5" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <autoFilter ref="G1:H5" xr:uid="{A722E349-13CC-4819-B8D7-4822A079EA8B}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{CAB148A1-4811-4744-ADA3-629C1D9783F6}" name="Punteggio" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{761918AF-30C9-4887-B56D-C4B26D78B52E}" name="Esito" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{CAB148A1-4811-4744-ADA3-629C1D9783F6}" name="Punteggio" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{761918AF-30C9-4887-B56D-C4B26D78B52E}" name="Esito" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>

</xml_diff>